<commit_message>
Update ER visit reduction Excel model
</commit_message>
<xml_diff>
--- a/excel-models/emergency_room_visit_reduction/emergency_room_visit_reduction.xlsx
+++ b/excel-models/emergency_room_visit_reduction/emergency_room_visit_reduction.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/da9bca8de754b386/Desktop/Applied Analytics/Case Study Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jack\OneDrive\Documents\Analytics-Portfolio\excel-models\emergency_room_visit_reduction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="764" documentId="8_{5FC079EC-8AF9-4582-96F5-9FB96D563A4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{61E4D96B-71EA-4F6A-A1CA-F70A726CF3AE}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C0E403A-6E48-4676-9365-629A3588D05E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27540" yWindow="615" windowWidth="27015" windowHeight="14760" xr2:uid="{224F360A-0BCC-4D10-A076-164AEB19AC52}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{224F360A-0BCC-4D10-A076-164AEB19AC52}"/>
   </bookViews>
   <sheets>
     <sheet name="Case Study Analysis" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="53">
   <si>
     <t>Membership</t>
   </si>
@@ -192,6 +192,9 @@
   </si>
   <si>
     <t>Summary</t>
+  </si>
+  <si>
+    <t>Option 2 Data</t>
   </si>
 </sst>
 </file>
@@ -401,7 +404,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -459,7 +462,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -514,10 +516,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -840,7 +838,7 @@
   <dimension ref="A1:Y35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -893,8 +891,6 @@
       <c r="R1" s="44"/>
       <c r="S1" s="44"/>
       <c r="T1" s="44"/>
-      <c r="U1" s="45"/>
-      <c r="V1" s="45"/>
     </row>
     <row r="2" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="23"/>
@@ -1388,6 +1384,17 @@
       </c>
       <c r="S12" s="1"/>
     </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="P14" s="44" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q14" s="44"/>
+      <c r="R14" s="44"/>
+      <c r="S14" s="44"/>
+      <c r="T14" s="44"/>
+      <c r="U14" s="44"/>
+      <c r="V14" s="44"/>
+    </row>
     <row r="15" spans="1:25" ht="48.75" x14ac:dyDescent="0.5">
       <c r="A15" s="43" t="s">
         <v>51</v>
@@ -1614,7 +1621,7 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="10">
     <mergeCell ref="A22:B22"/>
     <mergeCell ref="A15:B15"/>
     <mergeCell ref="P8:V8"/>
@@ -1624,6 +1631,7 @@
     <mergeCell ref="K1:N1"/>
     <mergeCell ref="A17:B17"/>
     <mergeCell ref="P1:T1"/>
+    <mergeCell ref="P14:V14"/>
   </mergeCells>
   <conditionalFormatting sqref="B18:B20">
     <cfRule type="cellIs" dxfId="3" priority="6" operator="equal">

</xml_diff>